<commit_message>
Lógica chegada de duplicados
</commit_message>
<xml_diff>
--- a/form4/expansao_atualizado_form4v2.xlsx
+++ b/form4/expansao_atualizado_form4v2.xlsx
@@ -3398,19 +3398,19 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="S28:T28"/>
     <mergeCell ref="O26:P26"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="R12:S12"/>
+    <mergeCell ref="C11:I11"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="M28:N28"/>
-    <mergeCell ref="K11:P11"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="M27:N27"/>
@@ -3438,7 +3438,7 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="K21:P21"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="K11:P11"/>
   </mergeCells>
   <conditionalFormatting sqref="T12">
     <cfRule type="cellIs" priority="5" operator="equal" dxfId="0">
@@ -59147,7 +59147,7 @@
     <col width="132" customWidth="1" min="8" max="8"/>
     <col width="34" customWidth="1" min="9" max="9"/>
     <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="92" customWidth="1" min="11" max="11"/>
+    <col width="95" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -59579,7 +59579,7 @@
       </c>
       <c r="K9" s="107" t="inlineStr">
         <is>
-          <t>Aguardando a Juliana voltar de férias para perguntar. A data parece ter sido corrigida.</t>
+          <t>Perguntar para a Diana se é para deletar mesmo. A data de envio parece ter sido corrigida.</t>
         </is>
       </c>
     </row>
@@ -61358,7 +61358,7 @@
       </c>
       <c r="F49" s="107" t="inlineStr">
         <is>
-          <t>05/05/2025, 08/04/2025</t>
+          <t>08/04/2025, 05/05/2025</t>
         </is>
       </c>
       <c r="G49" s="111" t="inlineStr">
@@ -65148,7 +65148,7 @@
       </c>
       <c r="F13" s="107" t="inlineStr">
         <is>
-          <t>10/07/2025, 09/06/2025</t>
+          <t>09/06/2025, 10/07/2025</t>
         </is>
       </c>
       <c r="G13" s="111" t="inlineStr">

</xml_diff>